<commit_message>
Sync Errors in Model
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\District_Heating_July22\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74C816B-1636-41F1-BD39-AADD4544E39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45D6C05-26BA-4590-8239-9E57B9B91076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-5415" yWindow="-15300" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="120">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -516,7 +516,10 @@
     <t>FT-RSDHET_3</t>
   </si>
   <si>
-    <t>UC_RHSRTS~0</t>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS</t>
   </si>
 </sst>
 </file>
@@ -529,11 +532,18 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -868,131 +878,132 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1008,16 +1019,20 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1033,12 +1048,13 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{BB0011A7-1A39-491F-B9B7-C0D5F250487E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D5D6510F-8CE0-49FB-8CB2-ED088CC704F4}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{813B4BDE-0070-4EDA-988A-7FE3A14EE573}"/>
+    <cellStyle name="Normal 3 2" xfId="6" xr:uid="{124214B4-3105-4EE3-A511-D47CF1EB98C0}"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2169,12 +2185,12 @@
       <c r="Z15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="15"/>
@@ -2258,11 +2274,11 @@
       <c r="A19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
@@ -2290,11 +2306,11 @@
       <c r="A20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
@@ -2322,11 +2338,11 @@
       <c r="A21" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
@@ -2352,9 +2368,9 @@
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
@@ -2382,11 +2398,11 @@
       <c r="A23" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -2412,11 +2428,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -2472,11 +2488,11 @@
       <c r="A26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -2502,11 +2518,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -2594,11 +2610,11 @@
       <c r="A30" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="12"/>
@@ -2626,11 +2642,11 @@
       <c r="A31" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="12"/>
@@ -5355,10 +5371,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AN14"/>
+  <dimension ref="A1:AO14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO9" sqref="AO9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5368,19 +5384,21 @@
     <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" style="1" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="52.7109375" style="1" customWidth="1"/>
-    <col min="12" max="40" width="8.7109375" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="55" customWidth="1"/>
+    <col min="9" max="10" width="8.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="62.85546875" style="1" customWidth="1"/>
+    <col min="13" max="41" width="8.7109375" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>106</v>
       </c>
@@ -5390,7 +5408,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -5422,8 +5440,9 @@
       <c r="AK4" s="4"/>
       <c r="AL4" s="4"/>
       <c r="AM4" s="4"/>
-    </row>
-    <row r="5" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="AN4" s="4"/>
+    </row>
+    <row r="5" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="43" t="s">
@@ -5433,10 +5452,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -5466,8 +5485,9 @@
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
-    </row>
-    <row r="6" spans="1:40" ht="15" x14ac:dyDescent="0.25">
+      <c r="AO5" s="4"/>
+    </row>
+    <row r="6" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="43" t="s">
@@ -5477,7 +5497,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -5510,19 +5530,20 @@
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO6" s="4"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="54"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -5553,8 +5574,9 @@
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
-    </row>
-    <row r="8" spans="1:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO7" s="4"/>
+    </row>
+    <row r="8" spans="1:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -5574,107 +5596,110 @@
       <c r="G8" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="J8" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="K8" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="L8" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="M8" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="N8" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="O8" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="44" t="s">
+      <c r="P8" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="44" t="s">
+      <c r="Q8" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="Q8" s="44" t="s">
+      <c r="R8" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="44" t="s">
+      <c r="S8" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="S8" s="44" t="s">
+      <c r="T8" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="44" t="s">
+      <c r="U8" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="U8" s="44" t="s">
+      <c r="V8" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="V8" s="44" t="s">
+      <c r="W8" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="W8" s="44" t="s">
+      <c r="X8" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="X8" s="44" t="s">
+      <c r="Y8" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="44" t="s">
+      <c r="Z8" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Z8" s="44" t="s">
+      <c r="AA8" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="AA8" s="44" t="s">
+      <c r="AB8" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="AB8" s="44" t="s">
+      <c r="AC8" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="AC8" s="44" t="s">
+      <c r="AD8" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="AD8" s="44" t="s">
+      <c r="AE8" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="AE8" s="44" t="s">
+      <c r="AF8" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="AF8" s="44" t="s">
+      <c r="AG8" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="AG8" s="44" t="s">
+      <c r="AH8" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="AH8" s="44" t="s">
+      <c r="AI8" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AI8" s="44" t="s">
+      <c r="AJ8" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="AJ8" s="44" t="s">
+      <c r="AK8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AK8" s="44" t="s">
+      <c r="AL8" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="AL8" s="44" t="s">
+      <c r="AM8" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="AM8" s="44" t="s">
+      <c r="AN8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="AN8" s="44" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AO8" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5692,134 +5717,137 @@
         <f>"RSDSH_"&amp;A9&amp;"*"</f>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="54">
+        <v>2019</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>-1</v>
       </c>
-      <c r="K9" s="4" t="str">
+      <c r="L9" s="4" t="str">
         <f>"Upper share of "&amp;A9&amp;" dwellings supplied by district heating in high density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in high density </v>
       </c>
-      <c r="L9" s="52">
-        <f>M9</f>
-        <v>5.1434483577431585E-2</v>
-      </c>
-      <c r="M9" s="53">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(M8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+      <c r="M9" s="52">
+        <f>N9</f>
         <v>5.1434483577431585E-2</v>
       </c>
       <c r="N9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.441860465116279E-2</v>
+        <v>5.1434483577431585E-2</v>
       </c>
       <c r="O9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.793624583694831E-2</v>
+        <v>7.441860465116279E-2</v>
       </c>
       <c r="P9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>0.10083782166367444</v>
+        <v>3.793624583694831E-2</v>
       </c>
       <c r="Q9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>8.0225988700564965E-2</v>
+        <v>0.10083782166367444</v>
       </c>
       <c r="R9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>0.1515527950310559</v>
+        <v>8.0225988700564965E-2</v>
       </c>
       <c r="S9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>5.0458715596330278E-2</v>
+        <v>0.1515527950310559</v>
       </c>
       <c r="T9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.3639891346526964E-2</v>
+        <v>5.0458715596330278E-2</v>
       </c>
       <c r="U9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>0.12007062978222484</v>
+        <v>6.3639891346526964E-2</v>
       </c>
       <c r="V9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.9525691699604744E-2</v>
+        <v>0.12007062978222484</v>
       </c>
       <c r="W9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.949044585987261E-2</v>
+        <v>3.9525691699604744E-2</v>
       </c>
       <c r="X9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>9.9173553719008267E-2</v>
+        <v>3.949044585987261E-2</v>
       </c>
       <c r="Y9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>9.9038118988243676E-2</v>
+        <v>9.9173553719008267E-2</v>
       </c>
       <c r="Z9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.7872744539411204E-2</v>
+        <v>9.9038118988243676E-2</v>
       </c>
       <c r="AA9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.241914618369987E-2</v>
+        <v>7.7872744539411204E-2</v>
       </c>
       <c r="AB9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>8.4169884169884177E-2</v>
+        <v>6.241914618369987E-2</v>
       </c>
       <c r="AC9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>4.0532365396249243E-2</v>
+        <v>8.4169884169884177E-2</v>
       </c>
       <c r="AD9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.18232044198895E-2</v>
+        <v>4.0532365396249243E-2</v>
       </c>
       <c r="AE9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.5067248273355138E-2</v>
+        <v>7.18232044198895E-2</v>
       </c>
       <c r="AF9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.4332909783989834E-2</v>
+        <v>6.5067248273355138E-2</v>
       </c>
       <c r="AG9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>8.3969465648854963E-2</v>
+        <v>7.4332909783989834E-2</v>
       </c>
       <c r="AH9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.4516129032258063E-2</v>
+        <v>8.3969465648854963E-2</v>
       </c>
       <c r="AI9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>2.5316455696202531E-2</v>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="AJ9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.5919540229885055E-2</v>
+        <v>2.5316455696202531E-2</v>
       </c>
       <c r="AK9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.3492063492063489E-2</v>
+        <v>3.5919540229885055E-2</v>
       </c>
       <c r="AL9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.0381231671554259E-2</v>
+        <v>6.3492063492063489E-2</v>
       </c>
       <c r="AM9" s="53">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>7.0381231671554259E-2</v>
+      </c>
+      <c r="AN9" s="53">
+        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5934065934065936E-2</v>
       </c>
-      <c r="AN9" s="49">
+      <c r="AO9" s="49">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -5837,134 +5865,137 @@
         <f>"RSDSH_"&amp;A10&amp;"*"</f>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
+      <c r="H10" s="54">
+        <v>2019</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>-1</v>
       </c>
-      <c r="K10" s="4" t="str">
+      <c r="L10" s="4" t="str">
         <f>"Upper share of "&amp;A10&amp;" dwellings supplied by district heating in medium density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
       </c>
-      <c r="L10" s="52">
-        <f>M10</f>
-        <v>0.16871353887503593</v>
-      </c>
-      <c r="M10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(M8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+      <c r="M10" s="52">
+        <f>N10</f>
         <v>0.16871353887503593</v>
       </c>
       <c r="N10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14050056882821388</v>
+        <v>0.16871353887503593</v>
       </c>
       <c r="O10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12740963855421686</v>
+        <v>0.14050056882821388</v>
       </c>
       <c r="P10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2127433090024331</v>
+        <v>0.12740963855421686</v>
       </c>
       <c r="Q10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17231638418079095</v>
+        <v>0.2127433090024331</v>
       </c>
       <c r="R10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.25650178480367158</v>
+        <v>0.17231638418079095</v>
       </c>
       <c r="S10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17156286721504113</v>
+        <v>0.25650178480367158</v>
       </c>
       <c r="T10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16129720503520376</v>
+        <v>0.17156286721504113</v>
       </c>
       <c r="U10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2263686304224285</v>
+        <v>0.16129720503520376</v>
       </c>
       <c r="V10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17887432536622977</v>
+        <v>0.2263686304224285</v>
       </c>
       <c r="W10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15068493150684931</v>
+        <v>0.17887432536622977</v>
       </c>
       <c r="X10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19209993247805537</v>
+        <v>0.15068493150684931</v>
       </c>
       <c r="Y10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.26583882412569693</v>
+        <v>0.19209993247805537</v>
       </c>
       <c r="Z10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2246203037569944</v>
+        <v>0.26583882412569693</v>
       </c>
       <c r="AA10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19334294640711366</v>
+        <v>0.2246203037569944</v>
       </c>
       <c r="AB10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.18867924528301888</v>
+        <v>0.19334294640711366</v>
       </c>
       <c r="AC10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14687859057832248</v>
+        <v>0.18867924528301888</v>
       </c>
       <c r="AD10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14393482196741098</v>
+        <v>0.14687859057832248</v>
       </c>
       <c r="AE10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19353940406571984</v>
+        <v>0.14393482196741098</v>
       </c>
       <c r="AF10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.21782023175696838</v>
+        <v>0.19353940406571984</v>
       </c>
       <c r="AG10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.30039525691699603</v>
+        <v>0.21782023175696838</v>
       </c>
       <c r="AH10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.184304932735426</v>
+        <v>0.30039525691699603</v>
       </c>
       <c r="AI10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.1189083820662768</v>
+        <v>0.184304932735426</v>
       </c>
       <c r="AJ10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15242494226327943</v>
+        <v>0.1189083820662768</v>
       </c>
       <c r="AK10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12763819095477386</v>
+        <v>0.15242494226327943</v>
       </c>
       <c r="AL10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.20583468395461912</v>
+        <v>0.12763819095477386</v>
       </c>
       <c r="AM10" s="51">
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.20583468395461912</v>
+      </c>
+      <c r="AN10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
         <v>7.0257611241217793E-2</v>
       </c>
-      <c r="AN10" s="49">
+      <c r="AO10" s="49">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -5982,134 +6013,137 @@
         <f>"RSDSH_"&amp;A11&amp;"*"</f>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
+      <c r="H11" s="54">
+        <v>2019</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>-1</v>
       </c>
-      <c r="K11" s="4" t="str">
+      <c r="L11" s="4" t="str">
         <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in low density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in low density </v>
       </c>
-      <c r="L11" s="52">
-        <f>M11</f>
-        <v>0.32876892584277057</v>
-      </c>
-      <c r="M11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(M8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="M11" s="52">
+        <f>N11</f>
         <v>0.32876892584277057</v>
       </c>
       <c r="N11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36983944954128439</v>
+        <v>0.32876892584277057</v>
       </c>
       <c r="O11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.19108471322294215</v>
+        <v>0.36983944954128439</v>
       </c>
       <c r="P11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30185089084933403</v>
+        <v>0.19108471322294215</v>
       </c>
       <c r="Q11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31262211801484957</v>
+        <v>0.30185089084933403</v>
       </c>
       <c r="R11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30314097881665447</v>
+        <v>0.31262211801484957</v>
       </c>
       <c r="S11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36356589147286822</v>
+        <v>0.30314097881665447</v>
       </c>
       <c r="T11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.34463702587289624</v>
+        <v>0.36356589147286822</v>
       </c>
       <c r="U11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32330598602248556</v>
+        <v>0.34463702587289624</v>
       </c>
       <c r="V11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.26618705035971224</v>
+        <v>0.32330598602248556</v>
       </c>
       <c r="W11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.24331870761866772</v>
+        <v>0.26618705035971224</v>
       </c>
       <c r="X11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.4841688654353562</v>
+        <v>0.24331870761866772</v>
       </c>
       <c r="Y11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.38530960140386061</v>
+        <v>0.4841688654353562</v>
       </c>
       <c r="Z11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31287219422812645</v>
+        <v>0.38530960140386061</v>
       </c>
       <c r="AA11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36640630497501936</v>
+        <v>0.31287219422812645</v>
       </c>
       <c r="AB11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.44163312248418629</v>
+        <v>0.36640630497501936</v>
       </c>
       <c r="AC11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.25227362593910635</v>
+        <v>0.44163312248418629</v>
       </c>
       <c r="AD11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.28832271762208067</v>
+        <v>0.25227362593910635</v>
       </c>
       <c r="AE11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.3616833431430253</v>
+        <v>0.28832271762208067</v>
       </c>
       <c r="AF11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.40211970074812969</v>
+        <v>0.3616833431430253</v>
       </c>
       <c r="AG11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.37364043506078054</v>
+        <v>0.40211970074812969</v>
       </c>
       <c r="AH11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36950286806883365</v>
+        <v>0.37364043506078054</v>
       </c>
       <c r="AI11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.35307621671258033</v>
+        <v>0.36950286806883365</v>
       </c>
       <c r="AJ11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32592592592592595</v>
+        <v>0.35307621671258033</v>
       </c>
       <c r="AK11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32150101419878296</v>
+        <v>0.32592592592592595</v>
       </c>
       <c r="AL11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.41375941948088196</v>
+        <v>0.32150101419878296</v>
       </c>
       <c r="AM11" s="51">
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.41375941948088196</v>
+      </c>
+      <c r="AN11" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.22955010224948874</v>
       </c>
-      <c r="AN11" s="49">
+      <c r="AO11" s="49">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -6119,11 +6153,11 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="54"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="50"/>
+      <c r="L12" s="4"/>
       <c r="M12" s="50"/>
       <c r="N12" s="50"/>
       <c r="O12" s="50"/>
@@ -6151,11 +6185,10 @@
       <c r="AK12" s="50"/>
       <c r="AL12" s="50"/>
       <c r="AM12" s="50"/>
-      <c r="AN12" s="49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="49"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -6165,12 +6198,12 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="54"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="47"/>
+      <c r="M13" s="4"/>
       <c r="N13" s="47"/>
       <c r="O13" s="47"/>
       <c r="P13" s="47"/>
@@ -6197,9 +6230,10 @@
       <c r="AK13" s="47"/>
       <c r="AL13" s="47"/>
       <c r="AM13" s="47"/>
-      <c r="AN13" s="4"/>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AN13" s="47"/>
+      <c r="AO13" s="4"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -6209,12 +6243,12 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="54"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="47"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="47"/>
       <c r="O14" s="47"/>
       <c r="P14" s="47"/>
@@ -6241,7 +6275,8 @@
       <c r="AK14" s="47"/>
       <c r="AL14" s="47"/>
       <c r="AM14" s="47"/>
-      <c r="AN14" s="4"/>
+      <c r="AN14" s="47"/>
+      <c r="AO14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6269,27 +6304,27 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="K4" s="58" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="K4" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="T4" s="58" t="s">
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="T4" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
@@ -8805,18 +8840,18 @@
     </row>
     <row r="3" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="63"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
@@ -10030,18 +10065,18 @@
     </row>
     <row r="34" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="61"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="63"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="33" t="s">
@@ -11238,18 +11273,18 @@
     </row>
     <row r="65" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="59" t="s">
+      <c r="B66" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="60"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="60"/>
-      <c r="J66" s="60"/>
-      <c r="K66" s="61"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="62"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="63"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="33" t="s">

</xml_diff>

<commit_message>
Sync error in limiting DH
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\District_Heating_July22\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45D6C05-26BA-4590-8239-9E57B9B91076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E88EDC-FAA1-4816-BE3A-910EADE023DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5415" yWindow="-15300" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -1015,10 +1015,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1046,6 +1042,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2185,12 +2185,12 @@
       <c r="Z15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="15"/>
@@ -2274,11 +2274,11 @@
       <c r="A19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
@@ -2306,11 +2306,11 @@
       <c r="A20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
@@ -2338,11 +2338,11 @@
       <c r="A21" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
@@ -2368,9 +2368,9 @@
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
@@ -2398,11 +2398,11 @@
       <c r="A23" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -2428,11 +2428,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -2488,11 +2488,11 @@
       <c r="A26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -2518,11 +2518,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -2610,11 +2610,11 @@
       <c r="A30" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="12"/>
@@ -2642,11 +2642,11 @@
       <c r="A31" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="12"/>
@@ -5371,10 +5371,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AO14"/>
+  <dimension ref="A1:AO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO9" sqref="AO9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5384,8 +5384,9 @@
     <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="8.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="55" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="53" customWidth="1"/>
     <col min="9" max="10" width="8.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="62.85546875" style="1" customWidth="1"/>
@@ -5408,7 +5409,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="54"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -5452,10 +5453,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -5497,7 +5498,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="54"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -5539,7 +5540,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="54"/>
+      <c r="H7" s="52"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
         <v>108</v>
@@ -5717,8 +5718,8 @@
         <f>"RSDSH_"&amp;A9&amp;"*"</f>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H9" s="54">
-        <v>2019</v>
+      <c r="H9" s="52">
+        <v>2018</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
@@ -5731,266 +5732,164 @@
         <f>"Upper share of "&amp;A9&amp;" dwellings supplied by district heating in high density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in high density </v>
       </c>
-      <c r="M9" s="52">
+      <c r="M9" s="62">
         <f>N9</f>
         <v>5.1434483577431585E-2</v>
       </c>
-      <c r="N9" s="53">
+      <c r="N9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>5.1434483577431585E-2</v>
       </c>
-      <c r="O9" s="53">
+      <c r="O9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.441860465116279E-2</v>
       </c>
-      <c r="P9" s="53">
+      <c r="P9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.793624583694831E-2</v>
       </c>
-      <c r="Q9" s="53">
+      <c r="Q9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.10083782166367444</v>
       </c>
-      <c r="R9" s="53">
+      <c r="R9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.0225988700564965E-2</v>
       </c>
-      <c r="S9" s="53">
+      <c r="S9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.1515527950310559</v>
       </c>
-      <c r="T9" s="53">
+      <c r="T9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>5.0458715596330278E-2</v>
       </c>
-      <c r="U9" s="53">
+      <c r="U9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.3639891346526964E-2</v>
       </c>
-      <c r="V9" s="53">
+      <c r="V9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.12007062978222484</v>
       </c>
-      <c r="W9" s="53">
+      <c r="W9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.9525691699604744E-2</v>
       </c>
-      <c r="X9" s="53">
+      <c r="X9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.949044585987261E-2</v>
       </c>
-      <c r="Y9" s="53">
+      <c r="Y9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>9.9173553719008267E-2</v>
       </c>
-      <c r="Z9" s="53">
+      <c r="Z9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>9.9038118988243676E-2</v>
       </c>
-      <c r="AA9" s="53">
+      <c r="AA9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.7872744539411204E-2</v>
       </c>
-      <c r="AB9" s="53">
+      <c r="AB9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.241914618369987E-2</v>
       </c>
-      <c r="AC9" s="53">
+      <c r="AC9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.4169884169884177E-2</v>
       </c>
-      <c r="AD9" s="53">
+      <c r="AD9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>4.0532365396249243E-2</v>
       </c>
-      <c r="AE9" s="53">
+      <c r="AE9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.18232044198895E-2</v>
       </c>
-      <c r="AF9" s="53">
+      <c r="AF9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5067248273355138E-2</v>
       </c>
-      <c r="AG9" s="53">
+      <c r="AG9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.4332909783989834E-2</v>
       </c>
-      <c r="AH9" s="53">
+      <c r="AH9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.3969465648854963E-2</v>
       </c>
-      <c r="AI9" s="53">
+      <c r="AI9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.4516129032258063E-2</v>
       </c>
-      <c r="AJ9" s="53">
+      <c r="AJ9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>2.5316455696202531E-2</v>
       </c>
-      <c r="AK9" s="53">
+      <c r="AK9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.5919540229885055E-2</v>
       </c>
-      <c r="AL9" s="53">
+      <c r="AL9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.3492063492063489E-2</v>
       </c>
-      <c r="AM9" s="53">
+      <c r="AM9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.0381231671554259E-2</v>
       </c>
-      <c r="AN9" s="53">
+      <c r="AN9" s="63">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5934065934065936E-2</v>
       </c>
       <c r="AO9" s="49">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="str">
-        <f>"DH_2_"&amp;A10&amp;"_UC"</f>
-        <v>DH_2_Det_UC</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="str">
-        <f>"RSDSH_"&amp;A10&amp;"*"</f>
-        <v>RSDSH_Det*</v>
-      </c>
-      <c r="H10" s="54">
-        <v>2019</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="4">
-        <v>-1</v>
-      </c>
-      <c r="L10" s="4" t="str">
-        <f>"Upper share of "&amp;A10&amp;" dwellings supplied by district heating in medium density "</f>
-        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
-      </c>
-      <c r="M10" s="52">
-        <f>N10</f>
-        <v>0.16871353887503593</v>
-      </c>
-      <c r="N10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16871353887503593</v>
-      </c>
-      <c r="O10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14050056882821388</v>
-      </c>
-      <c r="P10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12740963855421686</v>
-      </c>
-      <c r="Q10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2127433090024331</v>
-      </c>
-      <c r="R10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17231638418079095</v>
-      </c>
-      <c r="S10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.25650178480367158</v>
-      </c>
-      <c r="T10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17156286721504113</v>
-      </c>
-      <c r="U10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16129720503520376</v>
-      </c>
-      <c r="V10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2263686304224285</v>
-      </c>
-      <c r="W10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17887432536622977</v>
-      </c>
-      <c r="X10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15068493150684931</v>
-      </c>
-      <c r="Y10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19209993247805537</v>
-      </c>
-      <c r="Z10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.26583882412569693</v>
-      </c>
-      <c r="AA10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2246203037569944</v>
-      </c>
-      <c r="AB10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19334294640711366</v>
-      </c>
-      <c r="AC10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.18867924528301888</v>
-      </c>
-      <c r="AD10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14687859057832248</v>
-      </c>
-      <c r="AE10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14393482196741098</v>
-      </c>
-      <c r="AF10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19353940406571984</v>
-      </c>
-      <c r="AG10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.21782023175696838</v>
-      </c>
-      <c r="AH10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.30039525691699603</v>
-      </c>
-      <c r="AI10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.184304932735426</v>
-      </c>
-      <c r="AJ10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.1189083820662768</v>
-      </c>
-      <c r="AK10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15242494226327943</v>
-      </c>
-      <c r="AL10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12763819095477386</v>
-      </c>
-      <c r="AM10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.20583468395461912</v>
-      </c>
-      <c r="AN10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>7.0257611241217793E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52">
+        <v>0</v>
+      </c>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
+      <c r="Z10" s="63"/>
+      <c r="AA10" s="63"/>
+      <c r="AB10" s="63"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="63"/>
+      <c r="AE10" s="63"/>
+      <c r="AF10" s="63"/>
+      <c r="AG10" s="63"/>
+      <c r="AH10" s="63"/>
+      <c r="AI10" s="63"/>
+      <c r="AJ10" s="63"/>
+      <c r="AK10" s="63"/>
+      <c r="AL10" s="63"/>
+      <c r="AM10" s="63"/>
+      <c r="AN10" s="63"/>
       <c r="AO10" s="49">
         <v>5</v>
       </c>
@@ -6001,20 +5900,20 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="str">
-        <f>"DH_3_"&amp;A11&amp;"_UC"</f>
-        <v>DH_3_Det_UC</v>
+        <f>"DH_2_"&amp;A11&amp;"_UC"</f>
+        <v>DH_2_Det_UC</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="str">
         <f>"RSDSH_"&amp;A11&amp;"*"</f>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H11" s="54">
-        <v>2019</v>
+      <c r="H11" s="52">
+        <v>2018</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
@@ -6024,259 +5923,499 @@
         <v>-1</v>
       </c>
       <c r="L11" s="4" t="str">
-        <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in low density "</f>
-        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in low density </v>
-      </c>
-      <c r="M11" s="52">
+        <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in medium density "</f>
+        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
+      </c>
+      <c r="M11" s="62">
         <f>N11</f>
-        <v>0.32876892584277057</v>
+        <v>0.16871353887503593</v>
       </c>
       <c r="N11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32876892584277057</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.16871353887503593</v>
       </c>
       <c r="O11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36983944954128439</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14050056882821388</v>
       </c>
       <c r="P11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.19108471322294215</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.12740963855421686</v>
       </c>
       <c r="Q11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30185089084933403</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2127433090024331</v>
       </c>
       <c r="R11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31262211801484957</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17231638418079095</v>
       </c>
       <c r="S11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30314097881665447</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.25650178480367158</v>
       </c>
       <c r="T11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36356589147286822</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17156286721504113</v>
       </c>
       <c r="U11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.34463702587289624</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.16129720503520376</v>
       </c>
       <c r="V11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32330598602248556</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2263686304224285</v>
       </c>
       <c r="W11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.26618705035971224</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17887432536622977</v>
       </c>
       <c r="X11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.24331870761866772</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.15068493150684931</v>
       </c>
       <c r="Y11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.4841688654353562</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19209993247805537</v>
       </c>
       <c r="Z11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.38530960140386061</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.26583882412569693</v>
       </c>
       <c r="AA11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31287219422812645</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2246203037569944</v>
       </c>
       <c r="AB11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36640630497501936</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19334294640711366</v>
       </c>
       <c r="AC11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.44163312248418629</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.18867924528301888</v>
       </c>
       <c r="AD11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.25227362593910635</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14687859057832248</v>
       </c>
       <c r="AE11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.28832271762208067</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14393482196741098</v>
       </c>
       <c r="AF11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.3616833431430253</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19353940406571984</v>
       </c>
       <c r="AG11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.40211970074812969</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.21782023175696838</v>
       </c>
       <c r="AH11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.37364043506078054</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.30039525691699603</v>
       </c>
       <c r="AI11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36950286806883365</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.184304932735426</v>
       </c>
       <c r="AJ11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.35307621671258033</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.1189083820662768</v>
       </c>
       <c r="AK11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32592592592592595</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.15242494226327943</v>
       </c>
       <c r="AL11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32150101419878296</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.12763819095477386</v>
       </c>
       <c r="AM11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.41375941948088196</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.20583468395461912</v>
       </c>
       <c r="AN11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.22955010224948874</v>
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>7.0257611241217793E-2</v>
       </c>
       <c r="AO11" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52">
+        <v>0</v>
+      </c>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="51"/>
+      <c r="AA12" s="51"/>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="51"/>
+      <c r="AD12" s="51"/>
+      <c r="AE12" s="51"/>
+      <c r="AF12" s="51"/>
+      <c r="AG12" s="51"/>
+      <c r="AH12" s="51"/>
+      <c r="AI12" s="51"/>
+      <c r="AJ12" s="51"/>
+      <c r="AK12" s="51"/>
+      <c r="AL12" s="51"/>
+      <c r="AM12" s="51"/>
+      <c r="AN12" s="51"/>
+      <c r="AO12" s="49">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="50"/>
-      <c r="AB12" s="50"/>
-      <c r="AC12" s="50"/>
-      <c r="AD12" s="50"/>
-      <c r="AE12" s="50"/>
-      <c r="AF12" s="50"/>
-      <c r="AG12" s="50"/>
-      <c r="AH12" s="50"/>
-      <c r="AI12" s="50"/>
-      <c r="AJ12" s="50"/>
-      <c r="AK12" s="50"/>
-      <c r="AL12" s="50"/>
-      <c r="AM12" s="50"/>
-      <c r="AN12" s="50"/>
-      <c r="AO12" s="49"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="str">
+        <f>"DH_3_"&amp;A13&amp;"_UC"</f>
+        <v>DH_3_Det_UC</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="str">
+        <f>"RSDSH_"&amp;A13&amp;"*"</f>
+        <v>RSDSH_Det*</v>
+      </c>
+      <c r="H13" s="52">
+        <v>2018</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="4">
+        <v>-1</v>
+      </c>
+      <c r="L13" s="4" t="str">
+        <f>"Upper share of "&amp;A13&amp;" dwellings supplied by district heating in low density "</f>
+        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in low density </v>
+      </c>
+      <c r="M13" s="62">
+        <f>N13</f>
+        <v>0.32876892584277057</v>
+      </c>
+      <c r="N13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32876892584277057</v>
+      </c>
+      <c r="O13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36983944954128439</v>
+      </c>
+      <c r="P13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.19108471322294215</v>
+      </c>
+      <c r="Q13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.30185089084933403</v>
+      </c>
+      <c r="R13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.31262211801484957</v>
+      </c>
+      <c r="S13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.30314097881665447</v>
+      </c>
+      <c r="T13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36356589147286822</v>
+      </c>
+      <c r="U13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.34463702587289624</v>
+      </c>
+      <c r="V13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32330598602248556</v>
+      </c>
+      <c r="W13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.26618705035971224</v>
+      </c>
+      <c r="X13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.24331870761866772</v>
+      </c>
+      <c r="Y13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.4841688654353562</v>
+      </c>
+      <c r="Z13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.38530960140386061</v>
+      </c>
+      <c r="AA13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.31287219422812645</v>
+      </c>
+      <c r="AB13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36640630497501936</v>
+      </c>
+      <c r="AC13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.44163312248418629</v>
+      </c>
+      <c r="AD13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.25227362593910635</v>
+      </c>
+      <c r="AE13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.28832271762208067</v>
+      </c>
+      <c r="AF13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.3616833431430253</v>
+      </c>
+      <c r="AG13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.40211970074812969</v>
+      </c>
+      <c r="AH13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.37364043506078054</v>
+      </c>
+      <c r="AI13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36950286806883365</v>
+      </c>
+      <c r="AJ13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.35307621671258033</v>
+      </c>
+      <c r="AK13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32592592592592595</v>
+      </c>
+      <c r="AL13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32150101419878296</v>
+      </c>
+      <c r="AM13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.41375941948088196</v>
+      </c>
+      <c r="AN13" s="51">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.22955010224948874</v>
+      </c>
+      <c r="AO13" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52">
+        <v>0</v>
+      </c>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="51"/>
+      <c r="AI14" s="51"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="51"/>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="47"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="47"/>
-      <c r="U13" s="47"/>
-      <c r="V13" s="47"/>
-      <c r="W13" s="47"/>
-      <c r="X13" s="47"/>
-      <c r="Y13" s="47"/>
-      <c r="Z13" s="47"/>
-      <c r="AA13" s="47"/>
-      <c r="AB13" s="47"/>
-      <c r="AC13" s="47"/>
-      <c r="AD13" s="47"/>
-      <c r="AE13" s="47"/>
-      <c r="AF13" s="47"/>
-      <c r="AG13" s="47"/>
-      <c r="AH13" s="47"/>
-      <c r="AI13" s="47"/>
-      <c r="AJ13" s="47"/>
-      <c r="AK13" s="47"/>
-      <c r="AL13" s="47"/>
-      <c r="AM13" s="47"/>
-      <c r="AN13" s="47"/>
-      <c r="AO13" s="4"/>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="50"/>
+      <c r="Y15" s="50"/>
+      <c r="Z15" s="50"/>
+      <c r="AA15" s="50"/>
+      <c r="AB15" s="50"/>
+      <c r="AC15" s="50"/>
+      <c r="AD15" s="50"/>
+      <c r="AE15" s="50"/>
+      <c r="AF15" s="50"/>
+      <c r="AG15" s="50"/>
+      <c r="AH15" s="50"/>
+      <c r="AI15" s="50"/>
+      <c r="AJ15" s="50"/>
+      <c r="AK15" s="50"/>
+      <c r="AL15" s="50"/>
+      <c r="AM15" s="50"/>
+      <c r="AN15" s="50"/>
+      <c r="AO15" s="49"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="47"/>
-      <c r="R14" s="47"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="47"/>
-      <c r="U14" s="47"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="47"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
-      <c r="AH14" s="47"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="47"/>
-      <c r="AK14" s="47"/>
-      <c r="AL14" s="47"/>
-      <c r="AM14" s="47"/>
-      <c r="AN14" s="47"/>
-      <c r="AO14" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="47"/>
+      <c r="AC16" s="47"/>
+      <c r="AD16" s="47"/>
+      <c r="AE16" s="47"/>
+      <c r="AF16" s="47"/>
+      <c r="AG16" s="47"/>
+      <c r="AH16" s="47"/>
+      <c r="AI16" s="47"/>
+      <c r="AJ16" s="47"/>
+      <c r="AK16" s="47"/>
+      <c r="AL16" s="47"/>
+      <c r="AM16" s="47"/>
+      <c r="AN16" s="47"/>
+      <c r="AO16" s="4"/>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="47"/>
+      <c r="AH17" s="47"/>
+      <c r="AI17" s="47"/>
+      <c r="AJ17" s="47"/>
+      <c r="AK17" s="47"/>
+      <c r="AL17" s="47"/>
+      <c r="AM17" s="47"/>
+      <c r="AN17" s="47"/>
+      <c r="AO17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6304,27 +6443,27 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="K4" s="60" t="s">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="K4" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="T4" s="60" t="s">
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="T4" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="U4" s="60"/>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
@@ -8840,18 +8979,18 @@
     </row>
     <row r="3" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="63"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
@@ -10065,18 +10204,18 @@
     </row>
     <row r="34" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="63"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="61"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="33" t="s">
@@ -11273,18 +11412,18 @@
     </row>
     <row r="65" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="61" t="s">
+      <c r="B66" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="62"/>
-      <c r="D66" s="62"/>
-      <c r="E66" s="62"/>
-      <c r="F66" s="62"/>
-      <c r="G66" s="62"/>
-      <c r="H66" s="62"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="63"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="60"/>
+      <c r="I66" s="60"/>
+      <c r="J66" s="60"/>
+      <c r="K66" s="61"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="33" t="s">

</xml_diff>

<commit_message>
Synce errors and dummies
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E88EDC-FAA1-4816-BE3A-910EADE023DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC45555-5283-4CEB-8242-6028172471FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -1019,6 +1019,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1042,10 +1046,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2185,12 +2185,12 @@
       <c r="Z15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="15"/>
@@ -2274,11 +2274,11 @@
       <c r="A19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
@@ -2306,11 +2306,11 @@
       <c r="A20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
@@ -2338,11 +2338,11 @@
       <c r="A21" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
@@ -2368,9 +2368,9 @@
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
@@ -2398,11 +2398,11 @@
       <c r="A23" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -2428,11 +2428,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -2488,11 +2488,11 @@
       <c r="A26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -2518,11 +2518,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -2610,11 +2610,11 @@
       <c r="A30" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="12"/>
@@ -2642,11 +2642,11 @@
       <c r="A31" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="12"/>
@@ -5371,10 +5371,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AO17"/>
+  <dimension ref="A1:AO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO13" sqref="AO13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5732,164 +5732,266 @@
         <f>"Upper share of "&amp;A9&amp;" dwellings supplied by district heating in high density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in high density </v>
       </c>
-      <c r="M9" s="62">
+      <c r="M9" s="54">
         <f>N9</f>
         <v>5.1434483577431585E-2</v>
       </c>
-      <c r="N9" s="63">
+      <c r="N9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>5.1434483577431585E-2</v>
       </c>
-      <c r="O9" s="63">
+      <c r="O9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.441860465116279E-2</v>
       </c>
-      <c r="P9" s="63">
+      <c r="P9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.793624583694831E-2</v>
       </c>
-      <c r="Q9" s="63">
+      <c r="Q9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.10083782166367444</v>
       </c>
-      <c r="R9" s="63">
+      <c r="R9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.0225988700564965E-2</v>
       </c>
-      <c r="S9" s="63">
+      <c r="S9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.1515527950310559</v>
       </c>
-      <c r="T9" s="63">
+      <c r="T9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>5.0458715596330278E-2</v>
       </c>
-      <c r="U9" s="63">
+      <c r="U9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.3639891346526964E-2</v>
       </c>
-      <c r="V9" s="63">
+      <c r="V9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.12007062978222484</v>
       </c>
-      <c r="W9" s="63">
+      <c r="W9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.9525691699604744E-2</v>
       </c>
-      <c r="X9" s="63">
+      <c r="X9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.949044585987261E-2</v>
       </c>
-      <c r="Y9" s="63">
+      <c r="Y9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>9.9173553719008267E-2</v>
       </c>
-      <c r="Z9" s="63">
+      <c r="Z9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>9.9038118988243676E-2</v>
       </c>
-      <c r="AA9" s="63">
+      <c r="AA9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.7872744539411204E-2</v>
       </c>
-      <c r="AB9" s="63">
+      <c r="AB9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.241914618369987E-2</v>
       </c>
-      <c r="AC9" s="63">
+      <c r="AC9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.4169884169884177E-2</v>
       </c>
-      <c r="AD9" s="63">
+      <c r="AD9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>4.0532365396249243E-2</v>
       </c>
-      <c r="AE9" s="63">
+      <c r="AE9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.18232044198895E-2</v>
       </c>
-      <c r="AF9" s="63">
+      <c r="AF9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5067248273355138E-2</v>
       </c>
-      <c r="AG9" s="63">
+      <c r="AG9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.4332909783989834E-2</v>
       </c>
-      <c r="AH9" s="63">
+      <c r="AH9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.3969465648854963E-2</v>
       </c>
-      <c r="AI9" s="63">
+      <c r="AI9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.4516129032258063E-2</v>
       </c>
-      <c r="AJ9" s="63">
+      <c r="AJ9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>2.5316455696202531E-2</v>
       </c>
-      <c r="AK9" s="63">
+      <c r="AK9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.5919540229885055E-2</v>
       </c>
-      <c r="AL9" s="63">
+      <c r="AL9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.3492063492063489E-2</v>
       </c>
-      <c r="AM9" s="63">
+      <c r="AM9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.0381231671554259E-2</v>
       </c>
-      <c r="AN9" s="63">
+      <c r="AN9" s="55">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5934065934065936E-2</v>
       </c>
       <c r="AO9" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="str">
+        <f>"DH_2_"&amp;A10&amp;"_UC"</f>
+        <v>DH_2_Det_UC</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="str">
+        <f>"RSDSH_"&amp;A10&amp;"*"</f>
+        <v>RSDSH_Det*</v>
+      </c>
       <c r="H10" s="52">
-        <v>0</v>
-      </c>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="63"/>
-      <c r="S10" s="63"/>
-      <c r="T10" s="63"/>
-      <c r="U10" s="63"/>
-      <c r="V10" s="63"/>
-      <c r="W10" s="63"/>
-      <c r="X10" s="63"/>
-      <c r="Y10" s="63"/>
-      <c r="Z10" s="63"/>
-      <c r="AA10" s="63"/>
-      <c r="AB10" s="63"/>
-      <c r="AC10" s="63"/>
-      <c r="AD10" s="63"/>
-      <c r="AE10" s="63"/>
-      <c r="AF10" s="63"/>
-      <c r="AG10" s="63"/>
-      <c r="AH10" s="63"/>
-      <c r="AI10" s="63"/>
-      <c r="AJ10" s="63"/>
-      <c r="AK10" s="63"/>
-      <c r="AL10" s="63"/>
-      <c r="AM10" s="63"/>
-      <c r="AN10" s="63"/>
+        <v>2018</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="4">
+        <v>-1</v>
+      </c>
+      <c r="L10" s="4" t="str">
+        <f>"Upper share of "&amp;A10&amp;" dwellings supplied by district heating in medium density "</f>
+        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
+      </c>
+      <c r="M10" s="54">
+        <f>N10</f>
+        <v>0.16871353887503593</v>
+      </c>
+      <c r="N10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.16871353887503593</v>
+      </c>
+      <c r="O10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14050056882821388</v>
+      </c>
+      <c r="P10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.12740963855421686</v>
+      </c>
+      <c r="Q10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2127433090024331</v>
+      </c>
+      <c r="R10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17231638418079095</v>
+      </c>
+      <c r="S10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.25650178480367158</v>
+      </c>
+      <c r="T10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17156286721504113</v>
+      </c>
+      <c r="U10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.16129720503520376</v>
+      </c>
+      <c r="V10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2263686304224285</v>
+      </c>
+      <c r="W10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17887432536622977</v>
+      </c>
+      <c r="X10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.15068493150684931</v>
+      </c>
+      <c r="Y10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19209993247805537</v>
+      </c>
+      <c r="Z10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.26583882412569693</v>
+      </c>
+      <c r="AA10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2246203037569944</v>
+      </c>
+      <c r="AB10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19334294640711366</v>
+      </c>
+      <c r="AC10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.18867924528301888</v>
+      </c>
+      <c r="AD10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14687859057832248</v>
+      </c>
+      <c r="AE10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14393482196741098</v>
+      </c>
+      <c r="AF10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19353940406571984</v>
+      </c>
+      <c r="AG10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.21782023175696838</v>
+      </c>
+      <c r="AH10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.30039525691699603</v>
+      </c>
+      <c r="AI10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.184304932735426</v>
+      </c>
+      <c r="AJ10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.1189083820662768</v>
+      </c>
+      <c r="AK10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.15242494226327943</v>
+      </c>
+      <c r="AL10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.12763819095477386</v>
+      </c>
+      <c r="AM10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.20583468395461912</v>
+      </c>
+      <c r="AN10" s="51">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>7.0257611241217793E-2</v>
+      </c>
       <c r="AO10" s="49">
         <v>5</v>
       </c>
@@ -5900,12 +6002,12 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="str">
-        <f>"DH_2_"&amp;A11&amp;"_UC"</f>
-        <v>DH_2_Det_UC</v>
+        <f>"DH_3_"&amp;A11&amp;"_UC"</f>
+        <v>DH_3_Det_UC</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="str">
@@ -5923,123 +6025,123 @@
         <v>-1</v>
       </c>
       <c r="L11" s="4" t="str">
-        <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in medium density "</f>
-        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
-      </c>
-      <c r="M11" s="62">
+        <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in low density "</f>
+        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in low density </v>
+      </c>
+      <c r="M11" s="54">
         <f>N11</f>
-        <v>0.16871353887503593</v>
+        <v>0.32876892584277057</v>
       </c>
       <c r="N11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16871353887503593</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32876892584277057</v>
       </c>
       <c r="O11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14050056882821388</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36983944954128439</v>
       </c>
       <c r="P11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12740963855421686</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.19108471322294215</v>
       </c>
       <c r="Q11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2127433090024331</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.30185089084933403</v>
       </c>
       <c r="R11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17231638418079095</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.31262211801484957</v>
       </c>
       <c r="S11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.25650178480367158</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.30314097881665447</v>
       </c>
       <c r="T11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17156286721504113</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36356589147286822</v>
       </c>
       <c r="U11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16129720503520376</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.34463702587289624</v>
       </c>
       <c r="V11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2263686304224285</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32330598602248556</v>
       </c>
       <c r="W11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17887432536622977</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.26618705035971224</v>
       </c>
       <c r="X11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15068493150684931</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.24331870761866772</v>
       </c>
       <c r="Y11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19209993247805537</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.4841688654353562</v>
       </c>
       <c r="Z11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.26583882412569693</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.38530960140386061</v>
       </c>
       <c r="AA11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2246203037569944</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.31287219422812645</v>
       </c>
       <c r="AB11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19334294640711366</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36640630497501936</v>
       </c>
       <c r="AC11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.18867924528301888</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.44163312248418629</v>
       </c>
       <c r="AD11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14687859057832248</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.25227362593910635</v>
       </c>
       <c r="AE11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14393482196741098</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.28832271762208067</v>
       </c>
       <c r="AF11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19353940406571984</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.3616833431430253</v>
       </c>
       <c r="AG11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.21782023175696838</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.40211970074812969</v>
       </c>
       <c r="AH11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.30039525691699603</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.37364043506078054</v>
       </c>
       <c r="AI11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.184304932735426</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.36950286806883365</v>
       </c>
       <c r="AJ11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.1189083820662768</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.35307621671258033</v>
       </c>
       <c r="AK11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15242494226327943</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32592592592592595</v>
       </c>
       <c r="AL11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12763819095477386</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.32150101419878296</v>
       </c>
       <c r="AM11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.20583468395461912</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.41375941948088196</v>
       </c>
       <c r="AN11" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>7.0257611241217793E-2</v>
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>0.22955010224948874</v>
       </c>
       <c r="AO11" s="49">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
@@ -6049,14 +6151,12 @@
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
       <c r="G12" s="52"/>
-      <c r="H12" s="52">
-        <v>0</v>
-      </c>
+      <c r="H12" s="52"/>
       <c r="I12" s="52"/>
       <c r="J12" s="52"/>
       <c r="K12" s="52"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="62"/>
+      <c r="M12" s="54"/>
       <c r="N12" s="51"/>
       <c r="O12" s="51"/>
       <c r="P12" s="51"/>
@@ -6084,203 +6184,97 @@
       <c r="AL12" s="51"/>
       <c r="AM12" s="51"/>
       <c r="AN12" s="51"/>
-      <c r="AO12" s="49">
-        <v>5</v>
-      </c>
+      <c r="AO12" s="49"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="4" t="str">
-        <f>"DH_3_"&amp;A13&amp;"_UC"</f>
-        <v>DH_3_Det_UC</v>
-      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4" t="str">
-        <f>"RSDSH_"&amp;A13&amp;"*"</f>
-        <v>RSDSH_Det*</v>
-      </c>
-      <c r="H13" s="52">
-        <v>2018</v>
-      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="52"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="4">
-        <v>-1</v>
-      </c>
-      <c r="L13" s="4" t="str">
-        <f>"Upper share of "&amp;A13&amp;" dwellings supplied by district heating in low density "</f>
-        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in low density </v>
-      </c>
-      <c r="M13" s="62">
-        <f>N13</f>
-        <v>0.32876892584277057</v>
-      </c>
-      <c r="N13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32876892584277057</v>
-      </c>
-      <c r="O13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36983944954128439</v>
-      </c>
-      <c r="P13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.19108471322294215</v>
-      </c>
-      <c r="Q13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30185089084933403</v>
-      </c>
-      <c r="R13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31262211801484957</v>
-      </c>
-      <c r="S13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30314097881665447</v>
-      </c>
-      <c r="T13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36356589147286822</v>
-      </c>
-      <c r="U13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.34463702587289624</v>
-      </c>
-      <c r="V13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32330598602248556</v>
-      </c>
-      <c r="W13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.26618705035971224</v>
-      </c>
-      <c r="X13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.24331870761866772</v>
-      </c>
-      <c r="Y13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.4841688654353562</v>
-      </c>
-      <c r="Z13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.38530960140386061</v>
-      </c>
-      <c r="AA13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31287219422812645</v>
-      </c>
-      <c r="AB13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36640630497501936</v>
-      </c>
-      <c r="AC13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.44163312248418629</v>
-      </c>
-      <c r="AD13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.25227362593910635</v>
-      </c>
-      <c r="AE13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.28832271762208067</v>
-      </c>
-      <c r="AF13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.3616833431430253</v>
-      </c>
-      <c r="AG13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.40211970074812969</v>
-      </c>
-      <c r="AH13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.37364043506078054</v>
-      </c>
-      <c r="AI13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36950286806883365</v>
-      </c>
-      <c r="AJ13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.35307621671258033</v>
-      </c>
-      <c r="AK13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32592592592592595</v>
-      </c>
-      <c r="AL13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32150101419878296</v>
-      </c>
-      <c r="AM13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.41375941948088196</v>
-      </c>
-      <c r="AN13" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.22955010224948874</v>
-      </c>
-      <c r="AO13" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52">
-        <v>0</v>
-      </c>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="51"/>
-      <c r="AA14" s="51"/>
-      <c r="AB14" s="51"/>
-      <c r="AC14" s="51"/>
-      <c r="AD14" s="51"/>
-      <c r="AE14" s="51"/>
-      <c r="AF14" s="51"/>
-      <c r="AG14" s="51"/>
-      <c r="AH14" s="51"/>
-      <c r="AI14" s="51"/>
-      <c r="AJ14" s="51"/>
-      <c r="AK14" s="51"/>
-      <c r="AL14" s="51"/>
-      <c r="AM14" s="51"/>
-      <c r="AN14" s="51"/>
-      <c r="AO14" s="49">
-        <v>5</v>
-      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
+      <c r="AF13" s="50"/>
+      <c r="AG13" s="50"/>
+      <c r="AH13" s="50"/>
+      <c r="AI13" s="50"/>
+      <c r="AJ13" s="50"/>
+      <c r="AK13" s="50"/>
+      <c r="AL13" s="50"/>
+      <c r="AM13" s="50"/>
+      <c r="AN13" s="50"/>
+      <c r="AO13" s="49"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="47"/>
+      <c r="X14" s="47"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="47"/>
+      <c r="AD14" s="47"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
+      <c r="AG14" s="47"/>
+      <c r="AH14" s="47"/>
+      <c r="AI14" s="47"/>
+      <c r="AJ14" s="47"/>
+      <c r="AK14" s="47"/>
+      <c r="AL14" s="47"/>
+      <c r="AM14" s="47"/>
+      <c r="AN14" s="47"/>
+      <c r="AO14" s="4"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -6297,125 +6291,35 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="50"/>
-      <c r="AA15" s="50"/>
-      <c r="AB15" s="50"/>
-      <c r="AC15" s="50"/>
-      <c r="AD15" s="50"/>
-      <c r="AE15" s="50"/>
-      <c r="AF15" s="50"/>
-      <c r="AG15" s="50"/>
-      <c r="AH15" s="50"/>
-      <c r="AI15" s="50"/>
-      <c r="AJ15" s="50"/>
-      <c r="AK15" s="50"/>
-      <c r="AL15" s="50"/>
-      <c r="AM15" s="50"/>
-      <c r="AN15" s="50"/>
-      <c r="AO15" s="49"/>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="47"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="47"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="47"/>
-      <c r="Z16" s="47"/>
-      <c r="AA16" s="47"/>
-      <c r="AB16" s="47"/>
-      <c r="AC16" s="47"/>
-      <c r="AD16" s="47"/>
-      <c r="AE16" s="47"/>
-      <c r="AF16" s="47"/>
-      <c r="AG16" s="47"/>
-      <c r="AH16" s="47"/>
-      <c r="AI16" s="47"/>
-      <c r="AJ16" s="47"/>
-      <c r="AK16" s="47"/>
-      <c r="AL16" s="47"/>
-      <c r="AM16" s="47"/>
-      <c r="AN16" s="47"/>
-      <c r="AO16" s="4"/>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="47"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="47"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="47"/>
-      <c r="AA17" s="47"/>
-      <c r="AB17" s="47"/>
-      <c r="AC17" s="47"/>
-      <c r="AD17" s="47"/>
-      <c r="AE17" s="47"/>
-      <c r="AF17" s="47"/>
-      <c r="AG17" s="47"/>
-      <c r="AH17" s="47"/>
-      <c r="AI17" s="47"/>
-      <c r="AJ17" s="47"/>
-      <c r="AK17" s="47"/>
-      <c r="AL17" s="47"/>
-      <c r="AM17" s="47"/>
-      <c r="AN17" s="47"/>
-      <c r="AO17" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="47"/>
+      <c r="AD15" s="47"/>
+      <c r="AE15" s="47"/>
+      <c r="AF15" s="47"/>
+      <c r="AG15" s="47"/>
+      <c r="AH15" s="47"/>
+      <c r="AI15" s="47"/>
+      <c r="AJ15" s="47"/>
+      <c r="AK15" s="47"/>
+      <c r="AL15" s="47"/>
+      <c r="AM15" s="47"/>
+      <c r="AN15" s="47"/>
+      <c r="AO15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6443,27 +6347,27 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="K4" s="58" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="K4" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="T4" s="58" t="s">
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="T4" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
@@ -8979,18 +8883,18 @@
     </row>
     <row r="3" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="63"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
@@ -10204,18 +10108,18 @@
     </row>
     <row r="34" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="61"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="63"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="33" t="s">
@@ -11412,18 +11316,18 @@
     </row>
     <row r="65" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="59" t="s">
+      <c r="B66" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="60"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="60"/>
-      <c r="J66" s="60"/>
-      <c r="K66" s="61"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="62"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="63"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="33" t="s">

</xml_diff>

<commit_message>
Update after talk with Olex, DH limits and Urban density checks
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC45555-5283-4CEB-8242-6028172471FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3B6653-D818-4252-8E8F-42C806F3951C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="121">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -420,9 +420,6 @@
     <t>Limiting district heating to dwelling type</t>
   </si>
   <si>
-    <t>UP</t>
-  </si>
-  <si>
     <t>Data obtained from BER database in July 2022</t>
   </si>
   <si>
@@ -520,6 +517,12 @@
   </si>
   <si>
     <t>UC_RHSRTS</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS~0</t>
+  </si>
+  <si>
+    <t>LO</t>
   </si>
 </sst>
 </file>
@@ -887,7 +890,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1047,6 +1050,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -5371,10 +5379,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AO15"/>
+  <dimension ref="A1:AP15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5390,18 +5398,19 @@
     <col min="9" max="10" width="8.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="62.85546875" style="1" customWidth="1"/>
-    <col min="13" max="41" width="8.7109375" style="1" customWidth="1"/>
+    <col min="13" max="40" width="8.7109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="16" style="1" customWidth="1"/>
     <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -5443,11 +5452,11 @@
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
     </row>
-    <row r="5" spans="1:41" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -5488,7 +5497,7 @@
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
     </row>
-    <row r="6" spans="1:41" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="43" t="s">
@@ -5533,7 +5542,7 @@
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -5543,7 +5552,7 @@
       <c r="H7" s="52"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5577,7 +5586,7 @@
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
     </row>
-    <row r="8" spans="1:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -5586,28 +5595,28 @@
         <v>1</v>
       </c>
       <c r="D8" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="F8" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="G8" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="H8" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="46" t="s">
         <v>112</v>
-      </c>
-      <c r="H8" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="46" t="s">
-        <v>113</v>
       </c>
       <c r="J8" s="46" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L8" s="44" t="s">
         <v>3</v>
@@ -5696,11 +5705,14 @@
       <c r="AN8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="AO8" s="44" t="s">
+      <c r="AO8" s="46" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5711,7 +5723,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="str">
@@ -5722,8 +5734,8 @@
         <v>2018</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
-        <v>86</v>
+      <c r="J9" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="K9" s="4">
         <v>-1</v>
@@ -5844,11 +5856,14 @@
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5934065934065936E-2</v>
       </c>
-      <c r="AO9" s="49">
+      <c r="AO9" s="65">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -5859,7 +5874,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="str">
@@ -5870,8 +5885,8 @@
         <v>2018</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
-        <v>86</v>
+      <c r="J10" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="K10" s="4">
         <v>-1</v>
@@ -5992,11 +6007,14 @@
         <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
         <v>7.0257611241217793E-2</v>
       </c>
-      <c r="AO10" s="49">
+      <c r="AO10" s="65">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -6007,7 +6025,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="str">
@@ -6018,8 +6036,8 @@
         <v>2018</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
-        <v>86</v>
+      <c r="J11" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="K11" s="4">
         <v>-1</v>
@@ -6140,11 +6158,14 @@
         <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.22955010224948874</v>
       </c>
-      <c r="AO11" s="49">
+      <c r="AO11" s="65">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
@@ -6186,7 +6207,7 @@
       <c r="AN12" s="51"/>
       <c r="AO12" s="49"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -6231,7 +6252,7 @@
       <c r="AN13" s="50"/>
       <c r="AO13" s="49"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -6276,7 +6297,7 @@
       <c r="AN14" s="47"/>
       <c r="AO14" s="4"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -6332,7 +6353,7 @@
   <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T13" sqref="T13:AA13"/>
+      <selection activeCell="T11" sqref="T11:AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6343,26 +6364,33 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>87</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B4" s="60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
       <c r="E4" s="60"/>
       <c r="F4" s="60"/>
       <c r="K4" s="60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L4" s="60"/>
       <c r="M4" s="60"/>
       <c r="N4" s="60"/>
       <c r="O4" s="60"/>
       <c r="T4" s="60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U4" s="60"/>
       <c r="V4" s="60"/>
@@ -6371,19 +6399,19 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="D5" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="F5" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="G5" s="28" t="s">
         <v>5</v>
@@ -6395,19 +6423,19 @@
         <v>6</v>
       </c>
       <c r="K5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="M5" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="N5" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="N5" s="28" t="s">
+      <c r="O5" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="P5" s="28" t="s">
         <v>5</v>
@@ -6419,19 +6447,19 @@
         <v>6</v>
       </c>
       <c r="T5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="U5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="U5" s="28" t="s">
+      <c r="V5" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="W5" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="W5" s="28" t="s">
+      <c r="X5" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="X5" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="Y5" s="28" t="s">
         <v>5</v>
@@ -7506,7 +7534,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="30">
         <v>527</v>
@@ -7533,7 +7561,7 @@
         <v>0.25227362593910635</v>
       </c>
       <c r="K18" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L18" s="30">
         <v>595</v>
@@ -7560,7 +7588,7 @@
         <v>0.14687859057832248</v>
       </c>
       <c r="T18" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U18" s="30">
         <v>1801</v>
@@ -8386,7 +8414,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="30">
         <v>289</v>
@@ -8413,7 +8441,7 @@
         <v>0.3616833431430253</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L28" s="30">
         <v>410</v>
@@ -8440,7 +8468,7 @@
         <v>0.19353940406571984</v>
       </c>
       <c r="T28" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U28" s="30">
         <v>789</v>
@@ -8736,7 +8764,7 @@
         <v>66</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="30">
         <v>14623</v>
@@ -8763,7 +8791,7 @@
         <v>0.32876892584277057</v>
       </c>
       <c r="K32" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L32" s="30">
         <v>19886</v>
@@ -8790,7 +8818,7 @@
         <v>0.16871353887503593</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U32" s="30">
         <v>39496</v>
@@ -8867,7 +8895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1597DA-A015-4B01-A3B0-64DFC4C55D1A}">
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N91" sqref="N91"/>
     </sheetView>
   </sheetViews>
@@ -8878,13 +8906,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -8898,43 +8926,43 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="E5" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="F5" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="G5" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="H5" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="I5" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="J5" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="34" t="s">
-        <v>105</v>
-      </c>
       <c r="K5" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L5" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="M5" s="28" t="s">
-        <v>102</v>
-      </c>
       <c r="N5" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -9461,7 +9489,7 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="38">
         <v>6</v>
@@ -9901,7 +9929,7 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="38">
         <v>20</v>
@@ -10075,7 +10103,7 @@
     </row>
     <row r="32" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="41">
         <v>733</v>
@@ -10109,7 +10137,7 @@
     <row r="34" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="62"/>
       <c r="D35" s="62"/>
@@ -10123,43 +10151,43 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="E36" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="F36" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="G36" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G36" s="34" t="s">
+      <c r="H36" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="H36" s="34" t="s">
+      <c r="I36" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I36" s="34" t="s">
+      <c r="J36" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="J36" s="34" t="s">
-        <v>105</v>
-      </c>
       <c r="K36" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L36" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M36" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="M36" s="28" t="s">
-        <v>102</v>
-      </c>
       <c r="N36" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
@@ -10676,7 +10704,7 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B49" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" s="38">
         <v>17</v>
@@ -11108,7 +11136,7 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B59" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C59" s="38">
         <v>26</v>
@@ -11284,7 +11312,7 @@
     </row>
     <row r="63" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C63" s="41">
         <v>973</v>
@@ -11317,7 +11345,7 @@
     <row r="65" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B66" s="61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C66" s="62"/>
       <c r="D66" s="62"/>
@@ -11331,43 +11359,43 @@
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D67" s="34" t="s">
+      <c r="E67" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E67" s="34" t="s">
+      <c r="F67" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F67" s="34" t="s">
+      <c r="G67" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G67" s="34" t="s">
+      <c r="H67" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="H67" s="34" t="s">
+      <c r="I67" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I67" s="34" t="s">
+      <c r="J67" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="J67" s="34" t="s">
-        <v>105</v>
-      </c>
       <c r="K67" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L67" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M67" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="M67" s="28" t="s">
-        <v>102</v>
-      </c>
       <c r="N67" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
@@ -11874,7 +11902,7 @@
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B80" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C80" s="38">
         <v>39</v>
@@ -12282,7 +12310,7 @@
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B90" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C90" s="38">
         <v>6</v>
@@ -12454,7 +12482,7 @@
     </row>
     <row r="94" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B94" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C94" s="41">
         <v>2141</v>

</xml_diff>

<commit_message>
DH LHS not read by VEDA
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AC6501-12D4-4ABC-BCC2-49BE41061921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED173BF4-E048-47A5-92D2-788DEB63AB90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -480,9 +480,6 @@
     <t>UC - Each Region/Period</t>
   </si>
   <si>
-    <t>~UC_Sets: R_E:AllRegions</t>
-  </si>
-  <si>
     <t>~UC_T:UC_COMPRD</t>
   </si>
   <si>
@@ -523,6 +520,9 @@
   </si>
   <si>
     <t>LO</t>
+  </si>
+  <si>
+    <t>~UC_Sets: R_E:IE</t>
   </si>
 </sst>
 </file>
@@ -5381,8 +5381,8 @@
   </sheetPr>
   <dimension ref="A1:AP15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AN13" sqref="AN13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5457,7 +5457,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="43" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -5553,7 +5553,7 @@
       <c r="H7" s="52"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5596,28 +5596,28 @@
         <v>1</v>
       </c>
       <c r="D8" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="F8" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="G8" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="H8" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="46" t="s">
         <v>111</v>
-      </c>
-      <c r="H8" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="I8" s="46" t="s">
-        <v>112</v>
       </c>
       <c r="J8" s="46" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L8" s="44" t="s">
         <v>3</v>
@@ -5707,10 +5707,10 @@
         <v>26</v>
       </c>
       <c r="AO8" s="46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.2">
@@ -5724,7 +5724,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="52" t="str">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="I9" s="52"/>
       <c r="J9" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K9" s="4">
         <v>-1</v>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="52" t="str">
@@ -5887,7 +5887,7 @@
       </c>
       <c r="I10" s="52"/>
       <c r="J10" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K10" s="4">
         <v>-1</v>
@@ -6026,7 +6026,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="52" t="str">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="I11" s="52"/>
       <c r="J11" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K11" s="4">
         <v>-1</v>

</xml_diff>

<commit_message>
DH constraint not working
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED173BF4-E048-47A5-92D2-788DEB63AB90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EB44D1-C363-4528-A49F-200E3310DE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="120">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -516,9 +516,6 @@
     <t>UC_RHSRTS</t>
   </si>
   <si>
-    <t>UC_RHSRTS~0</t>
-  </si>
-  <si>
     <t>LO</t>
   </si>
   <si>
@@ -890,7 +887,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1009,9 +1006,6 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1027,9 +1021,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2193,12 +2184,12 @@
       <c r="Z15" s="12"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="15"/>
@@ -2282,11 +2273,11 @@
       <c r="A19" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
@@ -2314,11 +2305,11 @@
       <c r="A20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
@@ -2346,11 +2337,11 @@
       <c r="A21" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
@@ -2376,9 +2367,9 @@
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
@@ -2406,11 +2397,11 @@
       <c r="A23" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
@@ -2436,11 +2427,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -2496,11 +2487,11 @@
       <c r="A26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
@@ -2526,11 +2517,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -2618,11 +2609,11 @@
       <c r="A30" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="12"/>
@@ -2650,11 +2641,11 @@
       <c r="A31" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="12"/>
@@ -5379,10 +5370,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AP15"/>
+  <dimension ref="A1:AO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5394,22 +5385,21 @@
     <col min="5" max="5" width="26.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="53" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="52" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="62.85546875" style="1" customWidth="1"/>
     <col min="13" max="40" width="8.7109375" style="1" customWidth="1"/>
-    <col min="41" max="41" width="16" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="41" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
@@ -5419,7 +5409,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="52"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -5453,20 +5443,20 @@
       <c r="AM4" s="4"/>
       <c r="AN4" s="4"/>
     </row>
-    <row r="5" spans="1:42" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -5496,9 +5486,8 @@
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-    </row>
-    <row r="6" spans="1:42" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:41" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="43" t="s">
@@ -5507,8 +5496,8 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -5541,16 +5530,15 @@
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="52"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
         <v>106</v>
@@ -5585,9 +5573,8 @@
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
-      <c r="AO7" s="4"/>
-    </row>
-    <row r="8" spans="1:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -5706,14 +5693,11 @@
       <c r="AN8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="AO8" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="AP8" s="1" t="s">
+      <c r="AO8" s="44" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5727,16 +5711,16 @@
         <v>113</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="52" t="str">
+      <c r="G9" s="51" t="str">
         <f>"RSDSH_"&amp;A9&amp;"*"</f>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="51">
         <v>2018</v>
       </c>
-      <c r="I9" s="52"/>
-      <c r="J9" s="58" t="s">
-        <v>119</v>
+      <c r="I9" s="51"/>
+      <c r="J9" s="56" t="s">
+        <v>118</v>
       </c>
       <c r="K9" s="4">
         <v>-1</v>
@@ -5745,560 +5729,557 @@
         <f>"Upper share of "&amp;A9&amp;" dwellings supplied by district heating in high density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in high density </v>
       </c>
-      <c r="M9" s="54">
+      <c r="M9" s="53">
         <f>N9</f>
         <v>5.1434483577431585E-2</v>
       </c>
-      <c r="N9" s="55">
+      <c r="N9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>5.1434483577431585E-2</v>
       </c>
-      <c r="O9" s="55">
+      <c r="O9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.441860465116279E-2</v>
       </c>
-      <c r="P9" s="55">
+      <c r="P9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.793624583694831E-2</v>
       </c>
-      <c r="Q9" s="55">
+      <c r="Q9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.10083782166367444</v>
       </c>
-      <c r="R9" s="55">
+      <c r="R9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.0225988700564965E-2</v>
       </c>
-      <c r="S9" s="55">
+      <c r="S9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.1515527950310559</v>
       </c>
-      <c r="T9" s="55">
+      <c r="T9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>5.0458715596330278E-2</v>
       </c>
-      <c r="U9" s="55">
+      <c r="U9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.3639891346526964E-2</v>
       </c>
-      <c r="V9" s="55">
+      <c r="V9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>0.12007062978222484</v>
       </c>
-      <c r="W9" s="55">
+      <c r="W9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.9525691699604744E-2</v>
       </c>
-      <c r="X9" s="55">
+      <c r="X9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.949044585987261E-2</v>
       </c>
-      <c r="Y9" s="55">
+      <c r="Y9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>9.9173553719008267E-2</v>
       </c>
-      <c r="Z9" s="55">
+      <c r="Z9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>9.9038118988243676E-2</v>
       </c>
-      <c r="AA9" s="55">
+      <c r="AA9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.7872744539411204E-2</v>
       </c>
-      <c r="AB9" s="55">
+      <c r="AB9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.241914618369987E-2</v>
       </c>
-      <c r="AC9" s="55">
+      <c r="AC9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.4169884169884177E-2</v>
       </c>
-      <c r="AD9" s="55">
+      <c r="AD9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>4.0532365396249243E-2</v>
       </c>
-      <c r="AE9" s="55">
+      <c r="AE9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.18232044198895E-2</v>
       </c>
-      <c r="AF9" s="55">
+      <c r="AF9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5067248273355138E-2</v>
       </c>
-      <c r="AG9" s="55">
+      <c r="AG9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.4332909783989834E-2</v>
       </c>
-      <c r="AH9" s="55">
+      <c r="AH9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>8.3969465648854963E-2</v>
       </c>
-      <c r="AI9" s="55">
+      <c r="AI9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.4516129032258063E-2</v>
       </c>
-      <c r="AJ9" s="55">
+      <c r="AJ9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>2.5316455696202531E-2</v>
       </c>
-      <c r="AK9" s="55">
+      <c r="AK9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>3.5919540229885055E-2</v>
       </c>
-      <c r="AL9" s="55">
+      <c r="AL9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.3492063492063489E-2</v>
       </c>
-      <c r="AM9" s="55">
+      <c r="AM9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>7.0381231671554259E-2</v>
       </c>
-      <c r="AN9" s="55">
+      <c r="AN9" s="54">
         <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
         <v>6.5934065934065936E-2</v>
       </c>
-      <c r="AO9" s="57">
+      <c r="AO9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51">
+        <v>0</v>
+      </c>
+      <c r="I10" s="51"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
+      <c r="AB10" s="54"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="54"/>
+      <c r="AH10" s="54"/>
+      <c r="AI10" s="54"/>
+      <c r="AJ10" s="54"/>
+      <c r="AK10" s="54"/>
+      <c r="AL10" s="54"/>
+      <c r="AM10" s="54"/>
+      <c r="AN10" s="54"/>
+      <c r="AO10" s="52">
         <v>5</v>
       </c>
-      <c r="AP9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="str">
-        <f>"DH_2_"&amp;A10&amp;"_UC"</f>
-        <v>DH_2_Det_UC</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="52" t="str">
-        <f t="shared" ref="G10:G11" si="0">"RSDSH_"&amp;A10&amp;"*"</f>
-        <v>RSDSH_Det*</v>
-      </c>
-      <c r="H10" s="52">
-        <v>2018</v>
-      </c>
-      <c r="I10" s="52"/>
-      <c r="J10" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K10" s="4">
-        <v>-1</v>
-      </c>
-      <c r="L10" s="4" t="str">
-        <f>"Upper share of "&amp;A10&amp;" dwellings supplied by district heating in medium density "</f>
-        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
-      </c>
-      <c r="M10" s="54">
-        <f>N10</f>
-        <v>0.16871353887503593</v>
-      </c>
-      <c r="N10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16871353887503593</v>
-      </c>
-      <c r="O10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14050056882821388</v>
-      </c>
-      <c r="P10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12740963855421686</v>
-      </c>
-      <c r="Q10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2127433090024331</v>
-      </c>
-      <c r="R10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17231638418079095</v>
-      </c>
-      <c r="S10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.25650178480367158</v>
-      </c>
-      <c r="T10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17156286721504113</v>
-      </c>
-      <c r="U10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16129720503520376</v>
-      </c>
-      <c r="V10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2263686304224285</v>
-      </c>
-      <c r="W10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17887432536622977</v>
-      </c>
-      <c r="X10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15068493150684931</v>
-      </c>
-      <c r="Y10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19209993247805537</v>
-      </c>
-      <c r="Z10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.26583882412569693</v>
-      </c>
-      <c r="AA10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2246203037569944</v>
-      </c>
-      <c r="AB10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19334294640711366</v>
-      </c>
-      <c r="AC10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.18867924528301888</v>
-      </c>
-      <c r="AD10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14687859057832248</v>
-      </c>
-      <c r="AE10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14393482196741098</v>
-      </c>
-      <c r="AF10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19353940406571984</v>
-      </c>
-      <c r="AG10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.21782023175696838</v>
-      </c>
-      <c r="AH10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.30039525691699603</v>
-      </c>
-      <c r="AI10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.184304932735426</v>
-      </c>
-      <c r="AJ10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.1189083820662768</v>
-      </c>
-      <c r="AK10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15242494226327943</v>
-      </c>
-      <c r="AL10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12763819095477386</v>
-      </c>
-      <c r="AM10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.20583468395461912</v>
-      </c>
-      <c r="AN10" s="51">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>7.0257611241217793E-2</v>
-      </c>
-      <c r="AO10" s="57">
-        <v>5</v>
-      </c>
-      <c r="AP10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="str">
-        <f>"DH_3_"&amp;A11&amp;"_UC"</f>
-        <v>DH_3_Det_UC</v>
+        <f>"DH_2_"&amp;A11&amp;"_UC"</f>
+        <v>DH_2_Det_UC</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="51" t="str">
+        <f t="shared" ref="G11:G13" si="0">"RSDSH_"&amp;A11&amp;"*"</f>
+        <v>RSDSH_Det*</v>
+      </c>
+      <c r="H11" s="51">
+        <v>2018</v>
+      </c>
+      <c r="I11" s="51"/>
+      <c r="J11" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="4">
+        <v>-1</v>
+      </c>
+      <c r="L11" s="4" t="str">
+        <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in medium density "</f>
+        <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in medium density </v>
+      </c>
+      <c r="M11" s="53">
+        <f>N11</f>
+        <v>0.16871353887503593</v>
+      </c>
+      <c r="N11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.16871353887503593</v>
+      </c>
+      <c r="O11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14050056882821388</v>
+      </c>
+      <c r="P11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.12740963855421686</v>
+      </c>
+      <c r="Q11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2127433090024331</v>
+      </c>
+      <c r="R11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17231638418079095</v>
+      </c>
+      <c r="S11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.25650178480367158</v>
+      </c>
+      <c r="T11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17156286721504113</v>
+      </c>
+      <c r="U11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.16129720503520376</v>
+      </c>
+      <c r="V11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2263686304224285</v>
+      </c>
+      <c r="W11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.17887432536622977</v>
+      </c>
+      <c r="X11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.15068493150684931</v>
+      </c>
+      <c r="Y11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19209993247805537</v>
+      </c>
+      <c r="Z11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.26583882412569693</v>
+      </c>
+      <c r="AA11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.2246203037569944</v>
+      </c>
+      <c r="AB11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19334294640711366</v>
+      </c>
+      <c r="AC11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.18867924528301888</v>
+      </c>
+      <c r="AD11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14687859057832248</v>
+      </c>
+      <c r="AE11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.14393482196741098</v>
+      </c>
+      <c r="AF11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.19353940406571984</v>
+      </c>
+      <c r="AG11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.21782023175696838</v>
+      </c>
+      <c r="AH11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.30039525691699603</v>
+      </c>
+      <c r="AI11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.184304932735426</v>
+      </c>
+      <c r="AJ11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.1189083820662768</v>
+      </c>
+      <c r="AK11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.15242494226327943</v>
+      </c>
+      <c r="AL11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.12763819095477386</v>
+      </c>
+      <c r="AM11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>0.20583468395461912</v>
+      </c>
+      <c r="AN11" s="50">
+        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>7.0257611241217793E-2</v>
+      </c>
+      <c r="AO11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51">
+        <v>0</v>
+      </c>
+      <c r="I12" s="51"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
+      <c r="AC12" s="50"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AF12" s="50"/>
+      <c r="AG12" s="50"/>
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="str">
+        <f>"DH_3_"&amp;A13&amp;"_UC"</f>
+        <v>DH_3_Det_UC</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="52" t="str">
+      <c r="F13" s="4"/>
+      <c r="G13" s="51" t="str">
         <f t="shared" si="0"/>
         <v>RSDSH_Det*</v>
       </c>
-      <c r="H11" s="52">
+      <c r="H13" s="51">
         <v>2018</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K11" s="4">
+      <c r="I13" s="51"/>
+      <c r="J13" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="K13" s="4">
         <v>-1</v>
       </c>
-      <c r="L11" s="4" t="str">
-        <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in low density "</f>
+      <c r="L13" s="4" t="str">
+        <f>"Upper share of "&amp;A13&amp;" dwellings supplied by district heating in low density "</f>
         <v xml:space="preserve">Upper share of Det dwellings supplied by district heating in low density </v>
       </c>
-      <c r="M11" s="54">
-        <f>N11</f>
+      <c r="M13" s="53">
+        <f>N13</f>
         <v>0.32876892584277057</v>
       </c>
-      <c r="N11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="N13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(N8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.32876892584277057</v>
       </c>
-      <c r="O11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="O13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.36983944954128439</v>
       </c>
-      <c r="P11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="P13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.19108471322294215</v>
       </c>
-      <c r="Q11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="Q13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.30185089084933403</v>
       </c>
-      <c r="R11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="R13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.31262211801484957</v>
       </c>
-      <c r="S11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="S13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.30314097881665447</v>
       </c>
-      <c r="T11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="T13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.36356589147286822</v>
       </c>
-      <c r="U11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="U13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.34463702587289624</v>
       </c>
-      <c r="V11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="V13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.32330598602248556</v>
       </c>
-      <c r="W11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="W13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.26618705035971224</v>
       </c>
-      <c r="X11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="X13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.24331870761866772</v>
       </c>
-      <c r="Y11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="Y13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.4841688654353562</v>
       </c>
-      <c r="Z11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="Z13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.38530960140386061</v>
       </c>
-      <c r="AA11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AA13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.31287219422812645</v>
       </c>
-      <c r="AB11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AB13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.36640630497501936</v>
       </c>
-      <c r="AC11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AC13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.44163312248418629</v>
       </c>
-      <c r="AD11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AD13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.25227362593910635</v>
       </c>
-      <c r="AE11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AE13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.28832271762208067</v>
       </c>
-      <c r="AF11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AF13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.3616833431430253</v>
       </c>
-      <c r="AG11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AG13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.40211970074812969</v>
       </c>
-      <c r="AH11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AH13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.37364043506078054</v>
       </c>
-      <c r="AI11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AI13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.36950286806883365</v>
       </c>
-      <c r="AJ11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AJ13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.35307621671258033</v>
       </c>
-      <c r="AK11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AK13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.32592592592592595</v>
       </c>
-      <c r="AL11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AL13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.32150101419878296</v>
       </c>
-      <c r="AM11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AM13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.41375941948088196</v>
       </c>
-      <c r="AN11" s="51">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+      <c r="AN13" s="50">
+        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$13,Dwelling_Data!$G$5:$I$5,0))</f>
         <v>0.22955010224948874</v>
       </c>
-      <c r="AO11" s="57">
+      <c r="AO13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51">
+        <v>0</v>
+      </c>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="50"/>
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="50"/>
+      <c r="AC14" s="50"/>
+      <c r="AD14" s="50"/>
+      <c r="AE14" s="50"/>
+      <c r="AF14" s="50"/>
+      <c r="AG14" s="50"/>
+      <c r="AH14" s="50"/>
+      <c r="AI14" s="50"/>
+      <c r="AJ14" s="50"/>
+      <c r="AK14" s="50"/>
+      <c r="AL14" s="50"/>
+      <c r="AM14" s="50"/>
+      <c r="AN14" s="50"/>
+      <c r="AO14" s="52">
         <v>5</v>
       </c>
-      <c r="AP11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="51"/>
-      <c r="AB12" s="51"/>
-      <c r="AC12" s="51"/>
-      <c r="AD12" s="51"/>
-      <c r="AE12" s="51"/>
-      <c r="AF12" s="51"/>
-      <c r="AG12" s="51"/>
-      <c r="AH12" s="51"/>
-      <c r="AI12" s="51"/>
-      <c r="AJ12" s="51"/>
-      <c r="AK12" s="51"/>
-      <c r="AL12" s="51"/>
-      <c r="AM12" s="51"/>
-      <c r="AN12" s="51"/>
-      <c r="AO12" s="49"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="50"/>
-      <c r="AA13" s="50"/>
-      <c r="AB13" s="50"/>
-      <c r="AC13" s="50"/>
-      <c r="AD13" s="50"/>
-      <c r="AE13" s="50"/>
-      <c r="AF13" s="50"/>
-      <c r="AG13" s="50"/>
-      <c r="AH13" s="50"/>
-      <c r="AI13" s="50"/>
-      <c r="AJ13" s="50"/>
-      <c r="AK13" s="50"/>
-      <c r="AL13" s="50"/>
-      <c r="AM13" s="50"/>
-      <c r="AN13" s="50"/>
-      <c r="AO13" s="49"/>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="47"/>
-      <c r="R14" s="47"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="47"/>
-      <c r="U14" s="47"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="47"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
-      <c r="AH14" s="47"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="47"/>
-      <c r="AK14" s="47"/>
-      <c r="AL14" s="47"/>
-      <c r="AM14" s="47"/>
-      <c r="AN14" s="47"/>
-      <c r="AO14" s="4"/>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -6308,40 +6289,127 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="52"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
-      <c r="Q15" s="47"/>
-      <c r="R15" s="47"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="47"/>
-      <c r="U15" s="47"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="47"/>
-      <c r="X15" s="47"/>
-      <c r="Y15" s="47"/>
-      <c r="Z15" s="47"/>
-      <c r="AA15" s="47"/>
-      <c r="AB15" s="47"/>
-      <c r="AC15" s="47"/>
-      <c r="AD15" s="47"/>
-      <c r="AE15" s="47"/>
-      <c r="AF15" s="47"/>
-      <c r="AG15" s="47"/>
-      <c r="AH15" s="47"/>
-      <c r="AI15" s="47"/>
-      <c r="AJ15" s="47"/>
-      <c r="AK15" s="47"/>
-      <c r="AL15" s="47"/>
-      <c r="AM15" s="47"/>
-      <c r="AN15" s="47"/>
-      <c r="AO15" s="4"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="49"/>
+      <c r="AA15" s="49"/>
+      <c r="AB15" s="49"/>
+      <c r="AC15" s="49"/>
+      <c r="AD15" s="49"/>
+      <c r="AE15" s="49"/>
+      <c r="AF15" s="49"/>
+      <c r="AG15" s="49"/>
+      <c r="AH15" s="49"/>
+      <c r="AI15" s="49"/>
+      <c r="AJ15" s="49"/>
+      <c r="AK15" s="49"/>
+      <c r="AL15" s="49"/>
+      <c r="AM15" s="49"/>
+      <c r="AN15" s="49"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="47"/>
+      <c r="AC16" s="47"/>
+      <c r="AD16" s="47"/>
+      <c r="AE16" s="47"/>
+      <c r="AF16" s="47"/>
+      <c r="AG16" s="47"/>
+      <c r="AH16" s="47"/>
+      <c r="AI16" s="47"/>
+      <c r="AJ16" s="47"/>
+      <c r="AK16" s="47"/>
+      <c r="AL16" s="47"/>
+      <c r="AM16" s="47"/>
+      <c r="AN16" s="47"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="47"/>
+      <c r="AH17" s="47"/>
+      <c r="AI17" s="47"/>
+      <c r="AJ17" s="47"/>
+      <c r="AK17" s="47"/>
+      <c r="AL17" s="47"/>
+      <c r="AM17" s="47"/>
+      <c r="AN17" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6367,36 +6435,36 @@
       <c r="A1" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="K4" s="63" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="K4" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="T4" s="63" t="s">
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="T4" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="U4" s="63"/>
-      <c r="V4" s="63"/>
-      <c r="W4" s="63"/>
-      <c r="X4" s="63"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
@@ -8912,18 +8980,18 @@
     </row>
     <row r="3" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
@@ -10137,18 +10205,18 @@
     </row>
     <row r="34" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="66"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="64"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="33" t="s">
@@ -11345,18 +11413,18 @@
     </row>
     <row r="65" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="64" t="s">
+      <c r="B66" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="C66" s="65"/>
-      <c r="D66" s="65"/>
-      <c r="E66" s="65"/>
-      <c r="F66" s="65"/>
-      <c r="G66" s="65"/>
-      <c r="H66" s="65"/>
-      <c r="I66" s="65"/>
-      <c r="J66" s="65"/>
-      <c r="K66" s="66"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="63"/>
+      <c r="H66" s="63"/>
+      <c r="I66" s="63"/>
+      <c r="J66" s="63"/>
+      <c r="K66" s="64"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="33" t="s">

</xml_diff>

<commit_message>
test - not reading DH limit
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE2C5D0-D77A-470B-98FC-8CCCC8C2DBB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1E7CDD-0A12-45D4-A8B5-6C618518C027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="122">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -516,9 +516,6 @@
     <t>UC_RHSRTS</t>
   </si>
   <si>
-    <t>LO</t>
-  </si>
-  <si>
     <t>~UC_Sets: R_E:IE</t>
   </si>
   <si>
@@ -528,7 +525,7 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>~UC_T</t>
+    <t>UP</t>
   </si>
 </sst>
 </file>
@@ -5382,7 +5379,7 @@
   <dimension ref="A1:AQ15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5408,11 +5405,6 @@
     <row r="1" spans="1:43" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="K3" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
@@ -5463,12 +5455,12 @@
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="51"/>
       <c r="I5" s="51"/>
       <c r="K5" s="51"/>
@@ -5557,8 +5549,8 @@
       <c r="H7" s="51"/>
       <c r="I7" s="4"/>
       <c r="J7" s="51"/>
-      <c r="K7" s="4" t="s">
-        <v>122</v>
+      <c r="K7" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -5615,7 +5607,7 @@
         <v>111</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J8" s="46" t="s">
         <v>116</v>
@@ -5717,7 +5709,7 @@
         <v>117</v>
       </c>
       <c r="AQ8" s="44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.2">
@@ -5735,18 +5727,16 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="51" t="str">
-        <f>"RSDSH_"&amp;A9&amp;"*"</f>
-        <v>RSDSH_Det*</v>
+        <f>"RSD*H_"&amp;A9&amp;"*"</f>
+        <v>RSD*H_Det*</v>
       </c>
       <c r="I9" s="51"/>
-      <c r="J9" s="51">
-        <v>2018</v>
-      </c>
+      <c r="J9" s="51"/>
       <c r="K9" s="56" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L9" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M9" s="4" t="str">
         <f>"Upper share of "&amp;A9&amp;" dwellings supplied by district heating in high density "</f>
@@ -5754,115 +5744,115 @@
       </c>
       <c r="N9" s="53">
         <f>O9</f>
-        <v>5.1434483577431585E-2</v>
+        <v>-5.1434483577431585E-2</v>
       </c>
       <c r="O9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>5.1434483577431585E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-5.1434483577431585E-2</v>
       </c>
       <c r="P9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.441860465116279E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-7.441860465116279E-2</v>
       </c>
       <c r="Q9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.793624583694831E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-3.793624583694831E-2</v>
       </c>
       <c r="R9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>0.10083782166367444</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-0.10083782166367444</v>
       </c>
       <c r="S9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>8.0225988700564965E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-8.0225988700564965E-2</v>
       </c>
       <c r="T9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>0.1515527950310559</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-0.1515527950310559</v>
       </c>
       <c r="U9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>5.0458715596330278E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-5.0458715596330278E-2</v>
       </c>
       <c r="V9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.3639891346526964E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-6.3639891346526964E-2</v>
       </c>
       <c r="W9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>0.12007062978222484</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-0.12007062978222484</v>
       </c>
       <c r="X9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.9525691699604744E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-3.9525691699604744E-2</v>
       </c>
       <c r="Y9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.949044585987261E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-3.949044585987261E-2</v>
       </c>
       <c r="Z9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>9.9173553719008267E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-9.9173553719008267E-2</v>
       </c>
       <c r="AA9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>9.9038118988243676E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-9.9038118988243676E-2</v>
       </c>
       <c r="AB9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.7872744539411204E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-7.7872744539411204E-2</v>
       </c>
       <c r="AC9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.241914618369987E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-6.241914618369987E-2</v>
       </c>
       <c r="AD9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>8.4169884169884177E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-8.4169884169884177E-2</v>
       </c>
       <c r="AE9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>4.0532365396249243E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-4.0532365396249243E-2</v>
       </c>
       <c r="AF9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.18232044198895E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-7.18232044198895E-2</v>
       </c>
       <c r="AG9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.5067248273355138E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-6.5067248273355138E-2</v>
       </c>
       <c r="AH9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.4332909783989834E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-7.4332909783989834E-2</v>
       </c>
       <c r="AI9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>8.3969465648854963E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-8.3969465648854963E-2</v>
       </c>
       <c r="AJ9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.4516129032258063E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-6.4516129032258063E-2</v>
       </c>
       <c r="AK9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>2.5316455696202531E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-2.5316455696202531E-2</v>
       </c>
       <c r="AL9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>3.5919540229885055E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-3.5919540229885055E-2</v>
       </c>
       <c r="AM9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.3492063492063489E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-6.3492063492063489E-2</v>
       </c>
       <c r="AN9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>7.0381231671554259E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-7.0381231671554259E-2</v>
       </c>
       <c r="AO9" s="54">
-        <f>INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AO8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
-        <v>6.5934065934065936E-2</v>
+        <f>-INDEX(Dwelling_Data!$Y$6:$AA$32,MATCH(AO8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$9,Dwelling_Data!$Y$5:$AA$5,0))</f>
+        <v>-6.5934065934065936E-2</v>
       </c>
       <c r="AP9" s="1">
         <v>0</v>
@@ -5886,19 +5876,17 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="51" t="str">
-        <f t="shared" ref="G10:G11" si="0">"RSDSH_"&amp;A10&amp;"*"</f>
-        <v>RSDSH_Det*</v>
+        <f t="shared" ref="G10:G11" si="0">"RSD*H_"&amp;A10&amp;"*"</f>
+        <v>RSD*H_Det*</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="51"/>
-      <c r="J10" s="51">
-        <v>2018</v>
-      </c>
+      <c r="J10" s="51"/>
       <c r="K10" s="56" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L10" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M10" s="4" t="str">
         <f>"Upper share of "&amp;A10&amp;" dwellings supplied by district heating in medium density "</f>
@@ -5906,115 +5894,115 @@
       </c>
       <c r="N10" s="53">
         <f>O10</f>
-        <v>0.16871353887503593</v>
+        <v>-0.16871353887503593</v>
       </c>
       <c r="O10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16871353887503593</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.16871353887503593</v>
       </c>
       <c r="P10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14050056882821388</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.14050056882821388</v>
       </c>
       <c r="Q10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12740963855421686</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.12740963855421686</v>
       </c>
       <c r="R10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2127433090024331</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.2127433090024331</v>
       </c>
       <c r="S10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17231638418079095</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.17231638418079095</v>
       </c>
       <c r="T10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.25650178480367158</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.25650178480367158</v>
       </c>
       <c r="U10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17156286721504113</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.17156286721504113</v>
       </c>
       <c r="V10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.16129720503520376</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.16129720503520376</v>
       </c>
       <c r="W10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2263686304224285</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.2263686304224285</v>
       </c>
       <c r="X10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.17887432536622977</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.17887432536622977</v>
       </c>
       <c r="Y10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15068493150684931</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.15068493150684931</v>
       </c>
       <c r="Z10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19209993247805537</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.19209993247805537</v>
       </c>
       <c r="AA10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.26583882412569693</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.26583882412569693</v>
       </c>
       <c r="AB10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.2246203037569944</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.2246203037569944</v>
       </c>
       <c r="AC10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19334294640711366</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.19334294640711366</v>
       </c>
       <c r="AD10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.18867924528301888</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.18867924528301888</v>
       </c>
       <c r="AE10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14687859057832248</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.14687859057832248</v>
       </c>
       <c r="AF10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.14393482196741098</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.14393482196741098</v>
       </c>
       <c r="AG10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.19353940406571984</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.19353940406571984</v>
       </c>
       <c r="AH10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.21782023175696838</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.21782023175696838</v>
       </c>
       <c r="AI10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.30039525691699603</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.30039525691699603</v>
       </c>
       <c r="AJ10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.184304932735426</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.184304932735426</v>
       </c>
       <c r="AK10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.1189083820662768</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.1189083820662768</v>
       </c>
       <c r="AL10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.15242494226327943</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.15242494226327943</v>
       </c>
       <c r="AM10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.12763819095477386</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.12763819095477386</v>
       </c>
       <c r="AN10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>0.20583468395461912</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-0.20583468395461912</v>
       </c>
       <c r="AO10" s="50">
-        <f>INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AO8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
-        <v>7.0257611241217793E-2</v>
+        <f>-INDEX(Dwelling_Data!$P$6:$R$32,MATCH(AO8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$10,Dwelling_Data!$P$5:$R$5,0))</f>
+        <v>-7.0257611241217793E-2</v>
       </c>
       <c r="AP10" s="1">
         <v>0</v>
@@ -6039,18 +6027,16 @@
       <c r="F11" s="4"/>
       <c r="G11" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>RSDSH_Det*</v>
+        <v>RSD*H_Det*</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="51"/>
-      <c r="J11" s="51">
-        <v>2018</v>
-      </c>
+      <c r="J11" s="51"/>
       <c r="K11" s="56" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L11" s="4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M11" s="4" t="str">
         <f>"Upper share of "&amp;A11&amp;" dwellings supplied by district heating in low density "</f>
@@ -6058,115 +6044,115 @@
       </c>
       <c r="N11" s="53">
         <f>O11</f>
-        <v>0.32876892584277057</v>
+        <v>-0.32876892584277057</v>
       </c>
       <c r="O11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32876892584277057</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(O8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.32876892584277057</v>
       </c>
       <c r="P11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36983944954128439</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(P8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.36983944954128439</v>
       </c>
       <c r="Q11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.19108471322294215</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Q8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.19108471322294215</v>
       </c>
       <c r="R11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30185089084933403</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(R8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.30185089084933403</v>
       </c>
       <c r="S11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31262211801484957</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(S8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.31262211801484957</v>
       </c>
       <c r="T11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.30314097881665447</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(T8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.30314097881665447</v>
       </c>
       <c r="U11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36356589147286822</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(U8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.36356589147286822</v>
       </c>
       <c r="V11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.34463702587289624</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(V8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.34463702587289624</v>
       </c>
       <c r="W11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32330598602248556</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(W8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.32330598602248556</v>
       </c>
       <c r="X11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.26618705035971224</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(X8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.26618705035971224</v>
       </c>
       <c r="Y11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.24331870761866772</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Y8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.24331870761866772</v>
       </c>
       <c r="Z11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.4841688654353562</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(Z8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.4841688654353562</v>
       </c>
       <c r="AA11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.38530960140386061</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AA8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.38530960140386061</v>
       </c>
       <c r="AB11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.31287219422812645</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AB8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.31287219422812645</v>
       </c>
       <c r="AC11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36640630497501936</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AC8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.36640630497501936</v>
       </c>
       <c r="AD11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.44163312248418629</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AD8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.44163312248418629</v>
       </c>
       <c r="AE11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.25227362593910635</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AE8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.25227362593910635</v>
       </c>
       <c r="AF11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.28832271762208067</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AF8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.28832271762208067</v>
       </c>
       <c r="AG11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.3616833431430253</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AG8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.3616833431430253</v>
       </c>
       <c r="AH11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.40211970074812969</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AH8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.40211970074812969</v>
       </c>
       <c r="AI11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.37364043506078054</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AI8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.37364043506078054</v>
       </c>
       <c r="AJ11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.36950286806883365</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AJ8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.36950286806883365</v>
       </c>
       <c r="AK11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.35307621671258033</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AK8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.35307621671258033</v>
       </c>
       <c r="AL11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32592592592592595</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AL8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.32592592592592595</v>
       </c>
       <c r="AM11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.32150101419878296</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AM8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.32150101419878296</v>
       </c>
       <c r="AN11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.41375941948088196</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AN8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.41375941948088196</v>
       </c>
       <c r="AO11" s="50">
-        <f>INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AO8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
-        <v>0.22955010224948874</v>
+        <f>-INDEX(Dwelling_Data!$G$6:$I$32,MATCH(AO8,Dwelling_Data!$A$6:$A$32,0),MATCH($A$11,Dwelling_Data!$G$5:$I$5,0))</f>
+        <v>-0.22955010224948874</v>
       </c>
       <c r="AP11" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Error, DH UC not applied
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_DH_UC.xlsx
+++ b/SuppXLS/Scen_B_RSD_DH_UC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CD1054-DC75-448D-8143-43AFFC7A1A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE61ED4-AE91-4904-9E6E-FF77DB83B9EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="2670" yWindow="2610" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="123">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -529,9 +529,6 @@
   </si>
   <si>
     <t>~UC_Sets: R_E: IE</t>
-  </si>
-  <si>
-    <t>RSDHET</t>
   </si>
 </sst>
 </file>
@@ -5385,7 +5382,7 @@
   <dimension ref="A1:AQ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5736,9 +5733,7 @@
         <f>"R-S*_"&amp;A9&amp;"*"</f>
         <v>R-S*_Det*</v>
       </c>
-      <c r="H9" s="52" t="s">
-        <v>123</v>
-      </c>
+      <c r="H9" s="51"/>
       <c r="I9" s="51"/>
       <c r="J9" s="51">
         <v>2018</v>
@@ -5890,9 +5885,7 @@
         <f t="shared" ref="G10:G12" si="0">"R-S*_"&amp;A10&amp;"*"</f>
         <v>R-S*_Det*</v>
       </c>
-      <c r="H10" s="52" t="s">
-        <v>123</v>
-      </c>
+      <c r="H10" s="51"/>
       <c r="I10" s="51"/>
       <c r="J10" s="51">
         <v>2018</v>
@@ -6044,9 +6037,7 @@
         <f t="shared" si="0"/>
         <v>R-S*_Det*</v>
       </c>
-      <c r="H11" s="52" t="s">
-        <v>123</v>
-      </c>
+      <c r="H11" s="51"/>
       <c r="I11" s="51"/>
       <c r="J11" s="51">
         <v>2018</v>
@@ -6198,9 +6189,7 @@
         <f t="shared" si="0"/>
         <v>R-S*_Det*</v>
       </c>
-      <c r="H12" s="52" t="s">
-        <v>123</v>
-      </c>
+      <c r="H12" s="51"/>
       <c r="I12" s="51"/>
       <c r="J12" s="51">
         <v>2018</v>

</xml_diff>